<commit_message>
more blue forest story
</commit_message>
<xml_diff>
--- a/blue-forest-story/checklist.xlsx
+++ b/blue-forest-story/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/blue-forest-story/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Source/japanese-collectors-list/blue-forest-story/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07A73F72-5728-CA42-B005-B847823A840A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019049F6-596D-2445-8D24-C59FB4C29CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{387F16F3-7F95-2F48-A4CD-BE280C77B52C}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="25480" windowHeight="16360" xr2:uid="{387F16F3-7F95-2F48-A4CD-BE280C77B52C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>year</t>
   </si>
@@ -126,13 +126,46 @@
   </si>
   <si>
     <t>HG-085R</t>
+  </si>
+  <si>
+    <t>ブルーフォレスト通信3</t>
+  </si>
+  <si>
+    <t>Blue Forest Report 3</t>
+  </si>
+  <si>
+    <t>Grimpeur</t>
+  </si>
+  <si>
+    <t>blue_forest_report3.jpg</t>
+  </si>
+  <si>
+    <t>supplement</t>
+  </si>
+  <si>
+    <t>blue_forest_report.jpg</t>
+  </si>
+  <si>
+    <t>blue_forest_report2.jpg</t>
+  </si>
+  <si>
+    <t>ブルーフォレスト通信2</t>
+  </si>
+  <si>
+    <t>ブルーフォレスト通信</t>
+  </si>
+  <si>
+    <t>Blue Forest Report</t>
+  </si>
+  <si>
+    <t>Blue Forest Report 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +177,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -489,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F62593-6AEC-1049-A78A-CA7C2E536ACC}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F10" sqref="F8:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,7 +636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1996</v>
       </c>
@@ -657,7 +696,68 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2010</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2010</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2011</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>